<commit_message>
Linus' update to plate_layouts for 10/18/22 experiment
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/adp1-adaptation/plate_reader_screens/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C495F6-B2C6-304D-B67E-E93C279FD589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10747675-C4D8-7249-8033-E3B45C22359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38060" windowHeight="21860" activeTab="2" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.16" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="80">
   <si>
     <t>well</t>
   </si>
@@ -191,7 +191,91 @@
     <t>IPTG</t>
   </si>
   <si>
-    <t xml:space="preserve">NOT COMPLETE </t>
+    <t>compound _1</t>
+  </si>
+  <si>
+    <t>concentration_unit_1</t>
+  </si>
+  <si>
+    <t>concentration_1</t>
+  </si>
+  <si>
+    <t>compound_volume_1</t>
+  </si>
+  <si>
+    <t>compound_2</t>
+  </si>
+  <si>
+    <t>concentration_unit_2</t>
+  </si>
+  <si>
+    <t>concentration_2</t>
+  </si>
+  <si>
+    <t>compound_volume_2</t>
+  </si>
+  <si>
+    <t>pBWB163</t>
+  </si>
+  <si>
+    <t>pBWB164</t>
+  </si>
+  <si>
+    <t>Ampicilin</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
   </si>
 </sst>
 </file>
@@ -2589,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EA0AB2-4F32-6046-BCF2-3174397BF17B}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2609,682 +2693,1744 @@
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="3">
+        <v>250</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3">
+        <v>250</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="3">
+        <v>250</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="3">
+        <v>250</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="3">
+        <v>250</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="3">
+        <v>250</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="3">
+        <v>248</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="3">
+        <v>8</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="3">
+        <v>248</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="3">
+        <v>248</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
+      <c r="O10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="3">
+        <v>8</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="3">
+        <v>248</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3">
+        <v>8</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="3">
+        <v>248</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="3">
+        <v>8</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="3">
+        <v>248</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="3">
+        <v>10</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="3">
+        <v>8</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="3">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3">
+        <v>8</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2</v>
+      </c>
+      <c r="O16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="3">
+        <v>8</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="3">
+        <v>10</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="3">
+        <v>8</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1</v>
+      </c>
+      <c r="O18" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="3">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3">
+        <v>8</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="3">
+        <v>245.5</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2</v>
+      </c>
+      <c r="O19" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="3">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="3">
+        <v>8</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20" s="3">
+        <v>243</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="3">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="3">
+        <v>243</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="3">
+        <v>20</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="3">
+        <v>8</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22" s="3">
+        <v>243</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2</v>
+      </c>
+      <c r="O22" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="3">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3">
+        <v>5</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="3">
+        <v>8</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" s="3">
+        <v>243</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="3">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="3">
+        <v>8</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24" s="3">
+        <v>243</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1</v>
+      </c>
+      <c r="O24" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="3">
+        <v>20</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="3">
+        <v>8</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25" s="3">
+        <v>243</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N25" s="3">
+        <v>2</v>
+      </c>
+      <c r="O25" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2">
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="3">
+        <v>40</v>
+      </c>
+      <c r="F26" s="3">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="3">
+        <v>8</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="3">
+        <v>238</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="3">
+        <v>40</v>
+      </c>
+      <c r="F27" s="3">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="3">
+        <v>8</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27" s="3">
+        <v>238</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="3">
+        <v>40</v>
+      </c>
+      <c r="F28" s="3">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="3">
+        <v>8</v>
+      </c>
+      <c r="J28" s="3">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28" s="3">
+        <v>238</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2</v>
+      </c>
+      <c r="O28" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="3">
+        <v>40</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="3">
+        <v>8</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="3">
+        <v>238</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="3">
+        <v>40</v>
+      </c>
+      <c r="F30" s="3">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="3">
+        <v>8</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30" s="3">
+        <v>238</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+      <c r="O30" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="3">
+        <v>40</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31" s="3">
+        <v>238</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="3">
+        <v>2</v>
+      </c>
+      <c r="O31" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="3">
         <v>250</v>
       </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2">
+      <c r="F32" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="3">
+        <v>8</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="3">
         <v>0</v>
       </c>
-      <c r="K2" s="3">
+      <c r="O32" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="3">
+        <v>250</v>
+      </c>
+      <c r="F33" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="3">
+        <v>8</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" s="3">
+        <v>1</v>
+      </c>
+      <c r="O33" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="3">
+        <v>250</v>
+      </c>
+      <c r="F34" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="3">
+        <v>8</v>
+      </c>
+      <c r="J34" s="3">
+        <v>2</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2</v>
+      </c>
+      <c r="O34" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="3">
+        <v>250</v>
+      </c>
+      <c r="F35" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="3">
+        <v>8</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N35" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3">
+      <c r="O35" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="3">
         <v>250</v>
       </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3">
+      <c r="F36" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="3">
+        <v>8</v>
+      </c>
+      <c r="J36" s="3">
+        <v>2</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L36" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4">
+      <c r="O36" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="3">
         <v>250</v>
       </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="F37" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37" s="3">
+        <v>241.5</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N37" s="3">
+        <v>2</v>
+      </c>
+      <c r="O37" s="3">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5">
-        <v>250</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6">
-        <v>250</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7">
-        <v>250</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8">
-        <v>248</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9">
-        <v>248</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10">
-        <v>248</v>
-      </c>
-      <c r="I10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11">
-        <v>248</v>
-      </c>
-      <c r="I11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12">
-        <v>248</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13">
-        <v>248</v>
-      </c>
-      <c r="I13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14">
-        <v>225</v>
-      </c>
-      <c r="I14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15">
-        <v>225</v>
-      </c>
-      <c r="I15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16">
-        <v>225</v>
-      </c>
-      <c r="I16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17">
-        <v>225</v>
-      </c>
-      <c r="I17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>25</v>
-      </c>
-      <c r="G18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18">
-        <v>225</v>
-      </c>
-      <c r="I18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19">
-        <v>225</v>
-      </c>
-      <c r="I19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added data file changed plotting
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/circuit-state/plate-reader-screens/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linus\Desktop\BCCL\circuit-state\plate-reader-screens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10747675-C4D8-7249-8033-E3B45C22359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B1E180-5B35-4204-8F01-309C5377F8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38060" windowHeight="21860" activeTab="2" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.16" sheetId="6" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="78">
   <si>
     <t>well</t>
   </si>
@@ -213,12 +211,6 @@
   </si>
   <si>
     <t>compound_volume_2</t>
-  </si>
-  <si>
-    <t>pBWB163</t>
-  </si>
-  <si>
-    <t>pBWB164</t>
   </si>
   <si>
     <t>Ampicilin</t>
@@ -669,7 +661,7 @@
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
@@ -678,7 +670,7 @@
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -748,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -783,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -818,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -853,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -888,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -923,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -958,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -993,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1028,7 +1020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1063,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1098,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1133,7 +1125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1203,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1238,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1273,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1308,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1343,7 +1335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1378,7 +1370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1413,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1448,7 +1440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1483,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1518,7 +1510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1588,7 +1580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1623,7 +1615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1671,7 +1663,7 @@
       <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -1685,7 +1677,7 @@
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1720,7 +1712,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1755,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1825,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1860,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1895,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1930,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1965,7 +1957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2000,7 +1992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2035,7 +2027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2070,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2105,7 +2097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2140,7 +2132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2175,7 +2167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2210,7 +2202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2245,7 +2237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2280,7 +2272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2315,7 +2307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2350,7 +2342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2385,7 +2377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2420,7 +2412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2455,7 +2447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2490,7 +2482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2525,7 +2517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2560,7 +2552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2595,7 +2587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2630,7 +2622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2676,10 +2668,10 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -2693,7 +2685,7 @@
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2732,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2787,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2834,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2881,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2928,12 +2920,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>46</v>
@@ -2975,12 +2967,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>46</v>
@@ -3022,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3042,7 +3034,7 @@
         <v>46</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>42</v>
@@ -3069,7 +3061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -3089,7 +3081,7 @@
         <v>46</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>42</v>
@@ -3116,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -3136,7 +3128,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>42</v>
@@ -3163,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -3183,7 +3175,7 @@
         <v>46</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>42</v>
@@ -3210,7 +3202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -3230,7 +3222,7 @@
         <v>46</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>42</v>
@@ -3257,12 +3249,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>50</v>
@@ -3277,7 +3269,7 @@
         <v>46</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>42</v>
@@ -3304,7 +3296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -3324,7 +3316,7 @@
         <v>2.5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>42</v>
@@ -3351,7 +3343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -3371,7 +3363,7 @@
         <v>2.5</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>42</v>
@@ -3398,7 +3390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -3418,7 +3410,7 @@
         <v>2.5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>42</v>
@@ -3445,7 +3437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -3465,7 +3457,7 @@
         <v>2.5</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>42</v>
@@ -3492,7 +3484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -3512,7 +3504,7 @@
         <v>2.5</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>42</v>
@@ -3539,12 +3531,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>50</v>
@@ -3559,7 +3551,7 @@
         <v>2.5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>42</v>
@@ -3586,9 +3578,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>35</v>
@@ -3606,7 +3598,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>42</v>
@@ -3633,9 +3625,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>35</v>
@@ -3653,7 +3645,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>42</v>
@@ -3680,9 +3672,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>35</v>
@@ -3700,7 +3692,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>42</v>
@@ -3727,9 +3719,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>49</v>
@@ -3747,7 +3739,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>42</v>
@@ -3774,9 +3766,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>49</v>
@@ -3794,7 +3786,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>42</v>
@@ -3821,12 +3813,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>50</v>
@@ -3841,7 +3833,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>42</v>
@@ -3868,9 +3860,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>35</v>
@@ -3888,7 +3880,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>42</v>
@@ -3915,9 +3907,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
@@ -3935,7 +3927,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>42</v>
@@ -3962,9 +3954,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
@@ -3982,7 +3974,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>42</v>
@@ -4009,9 +4001,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>49</v>
@@ -4029,7 +4021,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>42</v>
@@ -4056,9 +4048,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>49</v>
@@ -4076,7 +4068,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>42</v>
@@ -4103,12 +4095,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>50</v>
@@ -4123,7 +4115,7 @@
         <v>10</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>42</v>
@@ -4150,9 +4142,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -4170,7 +4162,7 @@
         <v>6.25</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>42</v>
@@ -4197,9 +4189,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
@@ -4217,7 +4209,7 @@
         <v>6.25</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>42</v>
@@ -4244,9 +4236,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>35</v>
@@ -4264,7 +4256,7 @@
         <v>6.25</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>42</v>
@@ -4291,9 +4283,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>49</v>
@@ -4311,7 +4303,7 @@
         <v>6.25</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>42</v>
@@ -4338,9 +4330,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>49</v>
@@ -4358,7 +4350,7 @@
         <v>6.25</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>42</v>
@@ -4385,12 +4377,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>50</v>
@@ -4405,7 +4397,7 @@
         <v>6.25</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
more NAND analysis and figures for MSB paper
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/circuit-state/plate-reader-screens/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC6D8FC-8A1D-DA4D-8D99-5A7A775B1E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72474C98-FC6D-8140-97B7-62C9D6221DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="500" windowWidth="40040" windowHeight="27440" activeTab="3" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.12" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="80">
   <si>
     <t>well</t>
   </si>
@@ -268,16 +268,13 @@
     <t>MGZ1</t>
   </si>
   <si>
-    <t>dCASRx</t>
-  </si>
-  <si>
-    <t>mM</t>
-  </si>
-  <si>
     <t>compound_1</t>
   </si>
   <si>
     <t>wmedia</t>
+  </si>
+  <si>
+    <t>dCasRx</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>51</v>
@@ -4445,7 +4442,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4458,7 +4455,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>51</v>
@@ -4643,7 +4640,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -4690,7 +4687,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -4737,7 +4734,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -4796,7 +4793,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
@@ -4843,7 +4840,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
         <v>46</v>
@@ -4890,7 +4887,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
         <v>46</v>
@@ -4925,7 +4922,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -4937,7 +4934,7 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
         <v>46</v>
@@ -4972,7 +4969,7 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -4984,7 +4981,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
         <v>46</v>
@@ -5019,7 +5016,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -5031,7 +5028,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s">
         <v>46</v>
@@ -5078,13 +5075,13 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
         <v>50</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I14">
         <v>20</v>
@@ -5125,13 +5122,13 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
         <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I15">
         <v>20</v>
@@ -5172,13 +5169,13 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I16">
         <v>20</v>
@@ -5207,7 +5204,7 @@
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -5219,13 +5216,13 @@
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I17">
         <v>20</v>
@@ -5254,7 +5251,7 @@
         <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>41</v>
@@ -5266,13 +5263,13 @@
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
         <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I18">
         <v>20</v>
@@ -5301,7 +5298,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -5313,13 +5310,13 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
         <v>50</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="I19">
         <v>20</v>

</xml_diff>

<commit_message>
synthetic cell state biomarkers metadata
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72474C98-FC6D-8140-97B7-62C9D6221DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34912915-AD1F-8A46-AC23-63FF57E6BBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.12" sheetId="4" r:id="rId1"/>
     <sheet name="adp1_antibiotic_10.16" sheetId="6" r:id="rId2"/>
     <sheet name="adp1_antibiotic_10.18" sheetId="7" r:id="rId3"/>
     <sheet name="mgz1_antibiotic_11.9" sheetId="8" r:id="rId4"/>
+    <sheet name="168_antibiotic_11.19" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="87">
   <si>
     <t>well</t>
   </si>
@@ -275,6 +276,27 @@
   </si>
   <si>
     <t>dCasRx</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>4x</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E10</t>
   </si>
 </sst>
 </file>
@@ -4441,7 +4463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8075C6A6-247E-244C-9A0A-1989FC6E189D}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -5344,4 +5366,1001 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA40FCF-0912-E640-B95F-C99C753C7E17}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>168</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>250</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>250</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>250</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>250</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>250</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>250</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8">
+        <v>250</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>250</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10">
+        <v>250</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11">
+        <v>168</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11">
+        <v>250</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>168</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>2.5</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12">
+        <v>250</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>168</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13">
+        <v>250</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14">
+        <v>2.5</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14">
+        <v>250</v>
+      </c>
+      <c r="I14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>250</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>2.5</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16">
+        <v>250</v>
+      </c>
+      <c r="I16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>2.5</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>250</v>
+      </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18">
+        <v>2.5</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18">
+        <v>250</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19">
+        <v>2.5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19">
+        <v>250</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20">
+        <v>168</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20">
+        <v>250</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21">
+        <v>168</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21">
+        <v>250</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>168</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <v>250</v>
+      </c>
+      <c r="I22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23">
+        <v>250</v>
+      </c>
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24">
+        <v>250</v>
+      </c>
+      <c r="I24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25">
+        <v>250</v>
+      </c>
+      <c r="I25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26">
+        <v>250</v>
+      </c>
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27">
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28">
+        <v>250</v>
+      </c>
+      <c r="I28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new data and anticipate double titration data in plate layouts
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA0875B-018A-544F-B8D7-1FAF292A614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBDD9BA-978F-924E-B439-5D0D674BB319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1080" windowWidth="44120" windowHeight="25500" activeTab="8" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35980" windowHeight="27220" firstSheet="3" activeTab="9" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.12" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="mgDeltaLacI_mepMover_12.9.22" sheetId="11" r:id="rId7"/>
     <sheet name="mgDeltaLacI_mepMover_12.13.22" sheetId="13" r:id="rId8"/>
     <sheet name="mgDeltaLacI_mepMover_12.15.22" sheetId="14" r:id="rId9"/>
+    <sheet name="mgDeltaLacI_mepMover_12.22.22" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2907" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="130">
   <si>
     <t>well</t>
   </si>
@@ -512,6 +513,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA5F47"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1826,6 +1832,2845 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECD7123-BC65-B74D-9D41-4185F460C1BE}">
+  <dimension ref="A1:N61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>350</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>500</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <f>E2/2</f>
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>500</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="0">E3/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>43.75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>500</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>21.875</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>500</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>500</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>500</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>500</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>500</v>
+      </c>
+      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <v>500</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>350</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <f>I2/2</f>
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>500</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <f>E12/2</f>
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I21" si="1">I3/2</f>
+        <v>5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <v>500</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E21" si="2">E13/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>129</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>500</v>
+      </c>
+      <c r="M14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>43.75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15">
+        <v>500</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>21.875</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16">
+        <v>500</v>
+      </c>
+      <c r="M16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>500</v>
+      </c>
+      <c r="M17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18">
+        <v>500</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19">
+        <v>500</v>
+      </c>
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20">
+        <v>500</v>
+      </c>
+      <c r="M20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21">
+        <v>500</v>
+      </c>
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22">
+        <v>350</v>
+      </c>
+      <c r="F22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22">
+        <f>I12/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>129</v>
+      </c>
+      <c r="K22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22">
+        <v>500</v>
+      </c>
+      <c r="M22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <f>E22/2</f>
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I31" si="3">I13/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23">
+        <v>500</v>
+      </c>
+      <c r="M23" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E31" si="4">E23/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24">
+        <v>500</v>
+      </c>
+      <c r="M24" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>43.75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J25" t="s">
+        <v>129</v>
+      </c>
+      <c r="K25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25">
+        <v>500</v>
+      </c>
+      <c r="M25" t="s">
+        <v>40</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>21.875</v>
+      </c>
+      <c r="F26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>129</v>
+      </c>
+      <c r="K26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26">
+        <v>500</v>
+      </c>
+      <c r="M26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>129</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27">
+        <v>500</v>
+      </c>
+      <c r="M27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>129</v>
+      </c>
+      <c r="K28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28">
+        <v>500</v>
+      </c>
+      <c r="M28" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G29" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>129</v>
+      </c>
+      <c r="K29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29">
+        <v>500</v>
+      </c>
+      <c r="M29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F30" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J30" t="s">
+        <v>129</v>
+      </c>
+      <c r="K30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30">
+        <v>500</v>
+      </c>
+      <c r="M30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K31" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31">
+        <v>500</v>
+      </c>
+      <c r="M31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32">
+        <v>350</v>
+      </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32">
+        <f>I22/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="J32" t="s">
+        <v>129</v>
+      </c>
+      <c r="K32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32">
+        <v>500</v>
+      </c>
+      <c r="M32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <f>E32/2</f>
+        <v>175</v>
+      </c>
+      <c r="F33" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I41" si="5">I23/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="J33" t="s">
+        <v>129</v>
+      </c>
+      <c r="K33" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33">
+        <v>500</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E41" si="6">E33/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J34" t="s">
+        <v>129</v>
+      </c>
+      <c r="K34" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34">
+        <v>500</v>
+      </c>
+      <c r="M34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>43.75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J35" t="s">
+        <v>129</v>
+      </c>
+      <c r="K35" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35">
+        <v>500</v>
+      </c>
+      <c r="M35" t="s">
+        <v>40</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="6"/>
+        <v>21.875</v>
+      </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J36" t="s">
+        <v>129</v>
+      </c>
+      <c r="K36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L36">
+        <v>500</v>
+      </c>
+      <c r="M36" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="6"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F37" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" t="s">
+        <v>41</v>
+      </c>
+      <c r="H37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J37" t="s">
+        <v>129</v>
+      </c>
+      <c r="K37" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37">
+        <v>500</v>
+      </c>
+      <c r="M37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="6"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G38" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J38" t="s">
+        <v>129</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38">
+        <v>500</v>
+      </c>
+      <c r="M38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="6"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J39" t="s">
+        <v>129</v>
+      </c>
+      <c r="K39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39">
+        <v>500</v>
+      </c>
+      <c r="M39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="6"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F40" t="s">
+        <v>129</v>
+      </c>
+      <c r="G40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J40" t="s">
+        <v>129</v>
+      </c>
+      <c r="K40" t="s">
+        <v>38</v>
+      </c>
+      <c r="L40">
+        <v>500</v>
+      </c>
+      <c r="M40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="J41" t="s">
+        <v>129</v>
+      </c>
+      <c r="K41" t="s">
+        <v>38</v>
+      </c>
+      <c r="L41">
+        <v>500</v>
+      </c>
+      <c r="M41" t="s">
+        <v>40</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42">
+        <v>350</v>
+      </c>
+      <c r="F42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42">
+        <f>I32/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="J42" t="s">
+        <v>129</v>
+      </c>
+      <c r="K42" t="s">
+        <v>38</v>
+      </c>
+      <c r="L42">
+        <v>500</v>
+      </c>
+      <c r="M42" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43">
+        <f>E42/2</f>
+        <v>175</v>
+      </c>
+      <c r="F43" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" t="s">
+        <v>41</v>
+      </c>
+      <c r="H43" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43">
+        <f t="shared" ref="I43:I51" si="7">I33/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="J43" t="s">
+        <v>129</v>
+      </c>
+      <c r="K43" t="s">
+        <v>38</v>
+      </c>
+      <c r="L43">
+        <v>500</v>
+      </c>
+      <c r="M43" t="s">
+        <v>40</v>
+      </c>
+      <c r="N43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ref="E44:E51" si="8">E43/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" t="s">
+        <v>42</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J44" t="s">
+        <v>129</v>
+      </c>
+      <c r="K44" t="s">
+        <v>38</v>
+      </c>
+      <c r="L44">
+        <v>500</v>
+      </c>
+      <c r="M44" t="s">
+        <v>40</v>
+      </c>
+      <c r="N44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="8"/>
+        <v>43.75</v>
+      </c>
+      <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H45" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J45" t="s">
+        <v>129</v>
+      </c>
+      <c r="K45" t="s">
+        <v>38</v>
+      </c>
+      <c r="L45">
+        <v>500</v>
+      </c>
+      <c r="M45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="8"/>
+        <v>21.875</v>
+      </c>
+      <c r="F46" t="s">
+        <v>129</v>
+      </c>
+      <c r="G46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H46" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J46" t="s">
+        <v>129</v>
+      </c>
+      <c r="K46" t="s">
+        <v>38</v>
+      </c>
+      <c r="L46">
+        <v>500</v>
+      </c>
+      <c r="M46" t="s">
+        <v>40</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="8"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J47" t="s">
+        <v>129</v>
+      </c>
+      <c r="K47" t="s">
+        <v>38</v>
+      </c>
+      <c r="L47">
+        <v>500</v>
+      </c>
+      <c r="M47" t="s">
+        <v>40</v>
+      </c>
+      <c r="N47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="8"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J48" t="s">
+        <v>129</v>
+      </c>
+      <c r="K48" t="s">
+        <v>38</v>
+      </c>
+      <c r="L48">
+        <v>500</v>
+      </c>
+      <c r="M48" t="s">
+        <v>40</v>
+      </c>
+      <c r="N48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="8"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F49" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" t="s">
+        <v>41</v>
+      </c>
+      <c r="H49" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J49" t="s">
+        <v>129</v>
+      </c>
+      <c r="K49" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49">
+        <v>500</v>
+      </c>
+      <c r="M49" t="s">
+        <v>40</v>
+      </c>
+      <c r="N49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="8"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" t="s">
+        <v>42</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J50" t="s">
+        <v>129</v>
+      </c>
+      <c r="K50" t="s">
+        <v>38</v>
+      </c>
+      <c r="L50">
+        <v>500</v>
+      </c>
+      <c r="M50" t="s">
+        <v>40</v>
+      </c>
+      <c r="N50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>129</v>
+      </c>
+      <c r="G51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="J51" t="s">
+        <v>129</v>
+      </c>
+      <c r="K51" t="s">
+        <v>38</v>
+      </c>
+      <c r="L51">
+        <v>500</v>
+      </c>
+      <c r="M51" t="s">
+        <v>40</v>
+      </c>
+      <c r="N51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52">
+        <v>350</v>
+      </c>
+      <c r="F52" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" t="s">
+        <v>42</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>129</v>
+      </c>
+      <c r="K52" t="s">
+        <v>38</v>
+      </c>
+      <c r="L52">
+        <v>500</v>
+      </c>
+      <c r="M52" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53">
+        <f>E52/2</f>
+        <v>175</v>
+      </c>
+      <c r="F53" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>41</v>
+      </c>
+      <c r="H53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>129</v>
+      </c>
+      <c r="K53" t="s">
+        <v>38</v>
+      </c>
+      <c r="L53">
+        <v>500</v>
+      </c>
+      <c r="M53" t="s">
+        <v>40</v>
+      </c>
+      <c r="N53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54">
+        <f t="shared" ref="E54:E61" si="9">E53/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>129</v>
+      </c>
+      <c r="K54" t="s">
+        <v>38</v>
+      </c>
+      <c r="L54">
+        <v>500</v>
+      </c>
+      <c r="M54" t="s">
+        <v>40</v>
+      </c>
+      <c r="N54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="9"/>
+        <v>43.75</v>
+      </c>
+      <c r="F55" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55" t="s">
+        <v>41</v>
+      </c>
+      <c r="H55" t="s">
+        <v>42</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>129</v>
+      </c>
+      <c r="K55" t="s">
+        <v>38</v>
+      </c>
+      <c r="L55">
+        <v>500</v>
+      </c>
+      <c r="M55" t="s">
+        <v>40</v>
+      </c>
+      <c r="N55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="9"/>
+        <v>21.875</v>
+      </c>
+      <c r="F56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" t="s">
+        <v>42</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>129</v>
+      </c>
+      <c r="K56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L56">
+        <v>500</v>
+      </c>
+      <c r="M56" t="s">
+        <v>40</v>
+      </c>
+      <c r="N56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="9"/>
+        <v>10.9375</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" t="s">
+        <v>42</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>129</v>
+      </c>
+      <c r="K57" t="s">
+        <v>38</v>
+      </c>
+      <c r="L57">
+        <v>500</v>
+      </c>
+      <c r="M57" t="s">
+        <v>40</v>
+      </c>
+      <c r="N57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="9"/>
+        <v>5.46875</v>
+      </c>
+      <c r="F58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" t="s">
+        <v>41</v>
+      </c>
+      <c r="H58" t="s">
+        <v>42</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>129</v>
+      </c>
+      <c r="K58" t="s">
+        <v>38</v>
+      </c>
+      <c r="L58">
+        <v>500</v>
+      </c>
+      <c r="M58" t="s">
+        <v>40</v>
+      </c>
+      <c r="N58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="9"/>
+        <v>2.734375</v>
+      </c>
+      <c r="F59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" t="s">
+        <v>41</v>
+      </c>
+      <c r="H59" t="s">
+        <v>42</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>129</v>
+      </c>
+      <c r="K59" t="s">
+        <v>38</v>
+      </c>
+      <c r="L59">
+        <v>500</v>
+      </c>
+      <c r="M59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="9"/>
+        <v>1.3671875</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>129</v>
+      </c>
+      <c r="K60" t="s">
+        <v>38</v>
+      </c>
+      <c r="L60">
+        <v>500</v>
+      </c>
+      <c r="M60" t="s">
+        <v>40</v>
+      </c>
+      <c r="N60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" t="s">
+        <v>41</v>
+      </c>
+      <c r="H61" t="s">
+        <v>42</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>129</v>
+      </c>
+      <c r="K61" t="s">
+        <v>38</v>
+      </c>
+      <c r="L61">
+        <v>500</v>
+      </c>
+      <c r="M61" t="s">
+        <v>40</v>
+      </c>
+      <c r="N61">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="5"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color rgb="FFEA5F47"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F337F-D56F-DE4B-B44D-97EF61F12050}">
   <dimension ref="A1:K28"/>
@@ -10926,7 +13771,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:N61"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11033,7 +13878,8 @@
         <v>44</v>
       </c>
       <c r="E3">
-        <v>333.33330000000001</v>
+        <f>E2/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F3" t="s">
         <v>129</v>
@@ -11077,7 +13923,8 @@
         <v>44</v>
       </c>
       <c r="E4">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E4:E11" si="0">E3/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F4" t="s">
         <v>129</v>
@@ -11121,7 +13968,8 @@
         <v>44</v>
       </c>
       <c r="E5">
-        <v>37.036999999999999</v>
+        <f t="shared" si="0"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F5" t="s">
         <v>129</v>
@@ -11165,7 +14013,8 @@
         <v>44</v>
       </c>
       <c r="E6">
-        <v>12.345700000000001</v>
+        <f t="shared" si="0"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F6" t="s">
         <v>129</v>
@@ -11209,7 +14058,8 @@
         <v>44</v>
       </c>
       <c r="E7">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F7" t="s">
         <v>129</v>
@@ -11253,7 +14103,8 @@
         <v>44</v>
       </c>
       <c r="E8">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F8" t="s">
         <v>129</v>
@@ -11297,7 +14148,8 @@
         <v>44</v>
       </c>
       <c r="E9">
-        <v>0.4572</v>
+        <f t="shared" si="0"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F9" t="s">
         <v>129</v>
@@ -11341,7 +14193,8 @@
         <v>44</v>
       </c>
       <c r="E10">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F10" t="s">
         <v>129</v>
@@ -11385,7 +14238,8 @@
         <v>44</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F11" t="s">
         <v>129</v>
@@ -11473,7 +14327,8 @@
         <v>44</v>
       </c>
       <c r="E13">
-        <v>333.33330000000001</v>
+        <f>E12/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F13" t="s">
         <v>129</v>
@@ -11517,7 +14372,8 @@
         <v>44</v>
       </c>
       <c r="E14">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E14:E21" si="1">E13/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F14" t="s">
         <v>129</v>
@@ -11561,7 +14417,8 @@
         <v>44</v>
       </c>
       <c r="E15">
-        <v>37.036999999999999</v>
+        <f t="shared" si="1"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F15" t="s">
         <v>129</v>
@@ -11605,7 +14462,8 @@
         <v>44</v>
       </c>
       <c r="E16">
-        <v>12.345700000000001</v>
+        <f t="shared" si="1"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F16" t="s">
         <v>129</v>
@@ -11649,7 +14507,8 @@
         <v>44</v>
       </c>
       <c r="E17">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="1"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F17" t="s">
         <v>129</v>
@@ -11693,7 +14552,8 @@
         <v>44</v>
       </c>
       <c r="E18">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F18" t="s">
         <v>129</v>
@@ -11737,7 +14597,8 @@
         <v>44</v>
       </c>
       <c r="E19">
-        <v>0.4572</v>
+        <f t="shared" si="1"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F19" t="s">
         <v>129</v>
@@ -11781,7 +14642,8 @@
         <v>44</v>
       </c>
       <c r="E20">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F20" t="s">
         <v>129</v>
@@ -11825,7 +14687,8 @@
         <v>44</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F21" t="s">
         <v>129</v>
@@ -11913,7 +14776,8 @@
         <v>44</v>
       </c>
       <c r="E23">
-        <v>333.33330000000001</v>
+        <f>E22/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F23" t="s">
         <v>129</v>
@@ -11957,7 +14821,8 @@
         <v>44</v>
       </c>
       <c r="E24">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E24:E31" si="2">E23/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F24" t="s">
         <v>129</v>
@@ -12001,7 +14866,8 @@
         <v>44</v>
       </c>
       <c r="E25">
-        <v>37.036999999999999</v>
+        <f t="shared" si="2"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F25" t="s">
         <v>129</v>
@@ -12045,7 +14911,8 @@
         <v>44</v>
       </c>
       <c r="E26">
-        <v>12.345700000000001</v>
+        <f t="shared" si="2"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F26" t="s">
         <v>129</v>
@@ -12089,7 +14956,8 @@
         <v>44</v>
       </c>
       <c r="E27">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="2"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F27" t="s">
         <v>129</v>
@@ -12133,7 +15001,8 @@
         <v>44</v>
       </c>
       <c r="E28">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="2"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F28" t="s">
         <v>129</v>
@@ -12177,7 +15046,8 @@
         <v>44</v>
       </c>
       <c r="E29">
-        <v>0.4572</v>
+        <f t="shared" si="2"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F29" t="s">
         <v>129</v>
@@ -12221,7 +15091,8 @@
         <v>44</v>
       </c>
       <c r="E30">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F30" t="s">
         <v>129</v>
@@ -12265,7 +15136,8 @@
         <v>44</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F31" t="s">
         <v>129</v>
@@ -12353,7 +15225,8 @@
         <v>44</v>
       </c>
       <c r="E33">
-        <v>333.33330000000001</v>
+        <f>E32/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F33" t="s">
         <v>129</v>
@@ -12397,7 +15270,8 @@
         <v>44</v>
       </c>
       <c r="E34">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E34:E41" si="3">E33/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F34" t="s">
         <v>129</v>
@@ -12441,7 +15315,8 @@
         <v>44</v>
       </c>
       <c r="E35">
-        <v>37.036999999999999</v>
+        <f t="shared" si="3"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F35" t="s">
         <v>129</v>
@@ -12485,7 +15360,8 @@
         <v>44</v>
       </c>
       <c r="E36">
-        <v>12.345700000000001</v>
+        <f t="shared" si="3"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F36" t="s">
         <v>129</v>
@@ -12529,7 +15405,8 @@
         <v>44</v>
       </c>
       <c r="E37">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="3"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F37" t="s">
         <v>129</v>
@@ -12573,7 +15450,8 @@
         <v>44</v>
       </c>
       <c r="E38">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F38" t="s">
         <v>129</v>
@@ -12617,7 +15495,8 @@
         <v>44</v>
       </c>
       <c r="E39">
-        <v>0.4572</v>
+        <f t="shared" si="3"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F39" t="s">
         <v>129</v>
@@ -12661,7 +15540,8 @@
         <v>44</v>
       </c>
       <c r="E40">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F40" t="s">
         <v>129</v>
@@ -12705,7 +15585,8 @@
         <v>44</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F41" t="s">
         <v>129</v>
@@ -12793,7 +15674,8 @@
         <v>44</v>
       </c>
       <c r="E43">
-        <v>333.33330000000001</v>
+        <f>E42/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F43" t="s">
         <v>129</v>
@@ -12837,7 +15719,8 @@
         <v>44</v>
       </c>
       <c r="E44">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E44:E51" si="4">E43/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F44" t="s">
         <v>129</v>
@@ -12881,7 +15764,8 @@
         <v>44</v>
       </c>
       <c r="E45">
-        <v>37.036999999999999</v>
+        <f t="shared" si="4"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F45" t="s">
         <v>129</v>
@@ -12925,7 +15809,8 @@
         <v>44</v>
       </c>
       <c r="E46">
-        <v>12.345700000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F46" t="s">
         <v>129</v>
@@ -12969,7 +15854,8 @@
         <v>44</v>
       </c>
       <c r="E47">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="4"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F47" t="s">
         <v>129</v>
@@ -13013,7 +15899,8 @@
         <v>44</v>
       </c>
       <c r="E48">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="4"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F48" t="s">
         <v>129</v>
@@ -13057,7 +15944,8 @@
         <v>44</v>
       </c>
       <c r="E49">
-        <v>0.4572</v>
+        <f t="shared" si="4"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F49" t="s">
         <v>129</v>
@@ -13101,7 +15989,8 @@
         <v>44</v>
       </c>
       <c r="E50">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="4"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F50" t="s">
         <v>129</v>
@@ -13145,7 +16034,8 @@
         <v>44</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F51" t="s">
         <v>129</v>
@@ -13233,7 +16123,8 @@
         <v>44</v>
       </c>
       <c r="E53">
-        <v>333.33330000000001</v>
+        <f>E52/3</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="F53" t="s">
         <v>129</v>
@@ -13277,7 +16168,8 @@
         <v>44</v>
       </c>
       <c r="E54">
-        <v>111.11109999999999</v>
+        <f t="shared" ref="E54:E61" si="5">E53/3</f>
+        <v>111.1111111111111</v>
       </c>
       <c r="F54" t="s">
         <v>129</v>
@@ -13321,7 +16213,8 @@
         <v>44</v>
       </c>
       <c r="E55">
-        <v>37.036999999999999</v>
+        <f t="shared" si="5"/>
+        <v>37.037037037037031</v>
       </c>
       <c r="F55" t="s">
         <v>129</v>
@@ -13365,7 +16258,8 @@
         <v>44</v>
       </c>
       <c r="E56">
-        <v>12.345700000000001</v>
+        <f t="shared" si="5"/>
+        <v>12.345679012345677</v>
       </c>
       <c r="F56" t="s">
         <v>129</v>
@@ -13409,7 +16303,8 @@
         <v>44</v>
       </c>
       <c r="E57">
-        <v>4.1151999999999997</v>
+        <f t="shared" si="5"/>
+        <v>4.1152263374485587</v>
       </c>
       <c r="F57" t="s">
         <v>129</v>
@@ -13453,7 +16348,8 @@
         <v>44</v>
       </c>
       <c r="E58">
-        <v>1.3716999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.3717421124828528</v>
       </c>
       <c r="F58" t="s">
         <v>129</v>
@@ -13497,7 +16393,8 @@
         <v>44</v>
       </c>
       <c r="E59">
-        <v>0.4572</v>
+        <f t="shared" si="5"/>
+        <v>0.45724737082761763</v>
       </c>
       <c r="F59" t="s">
         <v>129</v>
@@ -13541,7 +16438,8 @@
         <v>44</v>
       </c>
       <c r="E60">
-        <v>0.15240000000000001</v>
+        <f t="shared" si="5"/>
+        <v>0.15241579027587254</v>
       </c>
       <c r="F60" t="s">
         <v>129</v>
@@ -13585,7 +16483,8 @@
         <v>44</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>5.0805263425290847E-2</v>
       </c>
       <c r="F61" t="s">
         <v>129</v>
@@ -13625,8 +16524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C776CA-D97E-A445-87E2-DE505312FDC8}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
double titration of iptg and amp analysis
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBDD9BA-978F-924E-B439-5D0D674BB319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78105C5B-DAC7-EF41-B623-78D024D25F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35980" windowHeight="27220" firstSheet="3" activeTab="9" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="4" activeTab="9" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.12" sheetId="4" r:id="rId1"/>
@@ -1836,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECD7123-BC65-B74D-9D41-4185F460C1BE}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,7 +1989,7 @@
         <v>44</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E11" si="0">E3/2</f>
+        <f t="shared" ref="E4:E10" si="0">E3/2</f>
         <v>87.5</v>
       </c>
       <c r="F4" t="s">
@@ -2331,7 +2331,7 @@
         <v>40</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -2439,7 +2439,7 @@
         <v>44</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E21" si="2">E13/2</f>
+        <f t="shared" ref="E14:E20" si="2">E13/2</f>
         <v>87.5</v>
       </c>
       <c r="F14" t="s">
@@ -2789,7 +2789,7 @@
         <v>40</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2897,7 +2897,7 @@
         <v>44</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E31" si="4">E23/2</f>
+        <f t="shared" ref="E24:E30" si="4">E23/2</f>
         <v>87.5</v>
       </c>
       <c r="F24" t="s">
@@ -3247,7 +3247,7 @@
         <v>40</v>
       </c>
       <c r="N31">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -3355,7 +3355,7 @@
         <v>44</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E41" si="6">E33/2</f>
+        <f t="shared" ref="E34:E40" si="6">E33/2</f>
         <v>87.5</v>
       </c>
       <c r="F34" t="s">
@@ -3705,7 +3705,7 @@
         <v>40</v>
       </c>
       <c r="N41">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -3813,7 +3813,7 @@
         <v>44</v>
       </c>
       <c r="E44">
-        <f t="shared" ref="E44:E51" si="8">E43/2</f>
+        <f t="shared" ref="E44:E50" si="8">E43/2</f>
         <v>87.5</v>
       </c>
       <c r="F44" t="s">
@@ -4163,7 +4163,7 @@
         <v>40</v>
       </c>
       <c r="N51">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -4269,7 +4269,7 @@
         <v>44</v>
       </c>
       <c r="E54">
-        <f t="shared" ref="E54:E61" si="9">E53/2</f>
+        <f t="shared" ref="E54:E60" si="9">E53/2</f>
         <v>87.5</v>
       </c>
       <c r="F54" t="s">
@@ -4611,7 +4611,7 @@
         <v>40</v>
       </c>
       <c r="N61">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -10251,7 +10251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91949FFA-5E6A-5C49-AD6E-C5C0E4B4C1C1}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
visualize latest mepM over results and biapenem / cefazolin screens
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF6CCED-7C0D-D94A-B02E-1194C6A62DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83421FC4-5C4F-EF4A-AD84-6454213E0546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="500" windowWidth="45080" windowHeight="26220" firstSheet="2" activeTab="12" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4559" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5062" uniqueCount="134">
   <si>
     <t>well</t>
   </si>
@@ -441,16 +441,13 @@
     <t>H9</t>
   </si>
   <si>
-    <t>11 ug/mL amp</t>
+    <t>MGZ1_mepM</t>
   </si>
   <si>
-    <t>5 uL of 0.5 mg/mL biapenem and cefazolin</t>
+    <t>biapenem</t>
   </si>
   <si>
-    <t>3 cols were wild type and 3 cols were with pMepMoverexpress and IPTG decreased going down the rows</t>
-  </si>
-  <si>
-    <t>Linus has the layout</t>
+    <t>cefazolin</t>
   </si>
 </sst>
 </file>
@@ -4696,7 +4693,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7068,7 +7065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D28DDB2-C3CD-B846-BE5F-AD48B0CE8247}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8738,7 +8737,7 @@
         <v>44</v>
       </c>
       <c r="E38">
-        <f>E37/5</f>
+        <f>E29/5</f>
         <v>0.47058823999999999</v>
       </c>
       <c r="F38" t="s">
@@ -8783,8 +8782,8 @@
         <v>44</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:E46" si="2">E38/5</f>
-        <v>9.4117647999999998E-2</v>
+        <f t="shared" ref="E39:E46" si="2">E30/5</f>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F39" t="s">
         <v>102</v>
@@ -8829,7 +8828,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>1.88235296E-2</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F40" t="s">
         <v>102</v>
@@ -8874,7 +8873,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>3.7647059199999999E-3</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F41" t="s">
         <v>102</v>
@@ -8919,7 +8918,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="2"/>
-        <v>7.5294118399999994E-4</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F42" t="s">
         <v>102</v>
@@ -8964,7 +8963,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="2"/>
-        <v>1.5058823679999999E-4</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F43" t="s">
         <v>102</v>
@@ -9009,7 +9008,7 @@
       </c>
       <c r="E44">
         <f t="shared" si="2"/>
-        <v>3.011764736E-5</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F44" t="s">
         <v>102</v>
@@ -9054,7 +9053,7 @@
       </c>
       <c r="E45">
         <f t="shared" si="2"/>
-        <v>6.0235294720000002E-6</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F45" t="s">
         <v>102</v>
@@ -9099,7 +9098,7 @@
       </c>
       <c r="E46">
         <f t="shared" si="2"/>
-        <v>1.2047058944E-6</v>
+        <v>0.47058823999999999</v>
       </c>
       <c r="F46" t="s">
         <v>102</v>
@@ -9191,36 +9190,2473 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0316DAE-8BCC-A846-AB6B-A7C3C6D5DDFD}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>5.5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>250</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>5.5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>250</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <f>E3/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <v>5.5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <f>E4/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>5.5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <f>E5/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>5.5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>250</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>5.5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>250</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>5.5</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>250</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <f>E8/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>11</v>
+      </c>
+      <c r="J9">
+        <v>5.5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>250</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <f>E9/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>5.5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>250</v>
+      </c>
+      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <f>E10/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <v>5.5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <v>250</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>5.5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>250</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>5.5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <f>E13/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>5.5</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+      <c r="M14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <f>E14/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <v>5.5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15">
+        <v>250</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <f>E15/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+      <c r="J16">
+        <v>5.5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16">
+        <v>250</v>
+      </c>
+      <c r="M16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" t="s">
+        <v>102</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>5.5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>5.5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18">
+        <v>250</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <f>E18/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>11</v>
+      </c>
+      <c r="J19">
+        <v>5.5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19">
+        <v>250</v>
+      </c>
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20">
+        <f>E19/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+      <c r="J20">
+        <v>5.5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20">
+        <v>250</v>
+      </c>
+      <c r="M20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" t="s">
+        <v>102</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <f>E20/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21">
+        <v>11</v>
+      </c>
+      <c r="J21">
+        <v>5.5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21">
+        <v>250</v>
+      </c>
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22">
+        <v>11</v>
+      </c>
+      <c r="J22">
+        <v>5.5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22">
+        <v>250</v>
+      </c>
+      <c r="M22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" t="s">
+        <v>102</v>
+      </c>
+      <c r="O22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23">
+        <v>11</v>
+      </c>
+      <c r="J23">
+        <v>5.5</v>
+      </c>
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23">
+        <v>250</v>
+      </c>
+      <c r="M23" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" t="s">
+        <v>102</v>
+      </c>
+      <c r="O23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24">
+        <f>E23/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24">
+        <v>11</v>
+      </c>
+      <c r="J24">
+        <v>5.5</v>
+      </c>
+      <c r="K24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24">
+        <v>250</v>
+      </c>
+      <c r="M24" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" t="s">
+        <v>102</v>
+      </c>
+      <c r="O24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <f>E24/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25">
+        <v>11</v>
+      </c>
+      <c r="J25">
+        <v>5.5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25">
+        <v>250</v>
+      </c>
+      <c r="M25" t="s">
+        <v>40</v>
+      </c>
+      <c r="N25" t="s">
+        <v>102</v>
+      </c>
+      <c r="O25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26">
+        <f>E25/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26">
+        <v>11</v>
+      </c>
+      <c r="J26">
+        <v>5.5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26">
+        <v>250</v>
+      </c>
+      <c r="M26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" t="s">
+        <v>102</v>
+      </c>
+      <c r="O26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <v>220.70588455999999</v>
+      </c>
+      <c r="F27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>5.5</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27">
+        <v>250</v>
+      </c>
+      <c r="M27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" t="s">
+        <v>102</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28">
+        <v>58.823529999999998</v>
+      </c>
+      <c r="F28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28">
+        <v>11</v>
+      </c>
+      <c r="J28">
+        <v>5.5</v>
+      </c>
+      <c r="K28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28">
+        <v>250</v>
+      </c>
+      <c r="M28" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" t="s">
+        <v>102</v>
+      </c>
+      <c r="O28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29">
+        <f>E28/5</f>
+        <v>11.764706</v>
+      </c>
+      <c r="F29" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29">
+        <v>11</v>
+      </c>
+      <c r="J29">
+        <v>5.5</v>
+      </c>
+      <c r="K29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29">
+        <v>250</v>
+      </c>
+      <c r="M29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N29" t="s">
+        <v>102</v>
+      </c>
+      <c r="O29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30">
+        <f>E29/5</f>
+        <v>2.3529412000000001</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30">
+        <v>11</v>
+      </c>
+      <c r="J30">
+        <v>5.5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30">
+        <v>250</v>
+      </c>
+      <c r="M30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" t="s">
+        <v>102</v>
+      </c>
+      <c r="O30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <f>E30/5</f>
+        <v>0.47058823999999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31">
+        <v>11</v>
+      </c>
+      <c r="J31">
+        <v>5.5</v>
+      </c>
+      <c r="K31" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31">
+        <v>250</v>
+      </c>
+      <c r="M31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32">
+        <v>250</v>
+      </c>
+      <c r="M32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33">
+        <v>250</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" t="s">
+        <v>102</v>
+      </c>
+      <c r="O33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34">
+        <v>250</v>
+      </c>
+      <c r="M34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N34" t="s">
+        <v>102</v>
+      </c>
+      <c r="O34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="K35" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35">
+        <v>250</v>
+      </c>
+      <c r="M35" t="s">
+        <v>40</v>
+      </c>
+      <c r="N35" t="s">
+        <v>102</v>
+      </c>
+      <c r="O35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L36">
+        <v>250</v>
+      </c>
+      <c r="M36" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36" t="s">
+        <v>102</v>
+      </c>
+      <c r="O36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37">
+        <v>250</v>
+      </c>
+      <c r="M37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N37" t="s">
+        <v>102</v>
+      </c>
+      <c r="O37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38">
+        <v>250</v>
+      </c>
+      <c r="M38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38" t="s">
+        <v>102</v>
+      </c>
+      <c r="O38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J39">
+        <v>5</v>
+      </c>
+      <c r="K39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39">
+        <v>250</v>
+      </c>
+      <c r="M39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" t="s">
+        <v>102</v>
+      </c>
+      <c r="O39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" t="s">
+        <v>133</v>
+      </c>
+      <c r="H40" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J40">
+        <v>5</v>
+      </c>
+      <c r="K40" t="s">
+        <v>38</v>
+      </c>
+      <c r="L40">
+        <v>250</v>
+      </c>
+      <c r="M40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N40" t="s">
+        <v>102</v>
+      </c>
+      <c r="O40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>102</v>
+      </c>
+      <c r="G41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" t="s">
+        <v>46</v>
+      </c>
+      <c r="K41" t="s">
+        <v>38</v>
+      </c>
+      <c r="L41">
+        <v>250</v>
+      </c>
+      <c r="M41" t="s">
+        <v>40</v>
+      </c>
+      <c r="N41" t="s">
+        <v>102</v>
+      </c>
+      <c r="O41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" t="s">
+        <v>46</v>
+      </c>
+      <c r="I42" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" t="s">
+        <v>46</v>
+      </c>
+      <c r="K42" t="s">
+        <v>38</v>
+      </c>
+      <c r="L42">
+        <v>250</v>
+      </c>
+      <c r="M42" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42" t="s">
+        <v>102</v>
+      </c>
+      <c r="O42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" t="s">
+        <v>46</v>
+      </c>
+      <c r="K43" t="s">
+        <v>38</v>
+      </c>
+      <c r="L43">
+        <v>250</v>
+      </c>
+      <c r="M43" t="s">
+        <v>40</v>
+      </c>
+      <c r="N43" t="s">
+        <v>102</v>
+      </c>
+      <c r="O43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" t="s">
         <v>132</v>
       </c>
-      <c r="E2" t="s">
-        <v>134</v>
+      <c r="H44" t="s">
+        <v>42</v>
+      </c>
+      <c r="I44">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="K44" t="s">
+        <v>38</v>
+      </c>
+      <c r="L44">
+        <v>250</v>
+      </c>
+      <c r="M44" t="s">
+        <v>40</v>
+      </c>
+      <c r="N44" t="s">
+        <v>102</v>
+      </c>
+      <c r="O44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" t="s">
+        <v>132</v>
+      </c>
+      <c r="H45" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J45">
+        <v>5</v>
+      </c>
+      <c r="K45" t="s">
+        <v>38</v>
+      </c>
+      <c r="L45">
+        <v>250</v>
+      </c>
+      <c r="M45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N45" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>102</v>
+      </c>
+      <c r="G46" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="K46" t="s">
+        <v>38</v>
+      </c>
+      <c r="L46">
+        <v>250</v>
+      </c>
+      <c r="M46" t="s">
+        <v>40</v>
+      </c>
+      <c r="N46" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>102</v>
+      </c>
+      <c r="G47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H47" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J47">
+        <v>5</v>
+      </c>
+      <c r="K47" t="s">
+        <v>38</v>
+      </c>
+      <c r="L47">
+        <v>250</v>
+      </c>
+      <c r="M47" t="s">
+        <v>40</v>
+      </c>
+      <c r="N47" t="s">
+        <v>102</v>
+      </c>
+      <c r="O47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J48">
+        <v>5</v>
+      </c>
+      <c r="K48" t="s">
+        <v>38</v>
+      </c>
+      <c r="L48">
+        <v>250</v>
+      </c>
+      <c r="M48" t="s">
+        <v>40</v>
+      </c>
+      <c r="N48" t="s">
+        <v>102</v>
+      </c>
+      <c r="O48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G49" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J49">
+        <v>5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49">
+        <v>250</v>
+      </c>
+      <c r="M49" t="s">
+        <v>40</v>
+      </c>
+      <c r="N49" t="s">
+        <v>102</v>
+      </c>
+      <c r="O49">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I1:I31">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E2 E4:E6">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11 E7">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E16 E12">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:E21 E17">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E26 E22">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E31 E27">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
incorporate logreg results in downstream analysis
</commit_message>
<xml_diff>
--- a/plate-reader-screens/plate_layouts.xlsx
+++ b/plate-reader-screens/plate_layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/plate-reader-screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83421FC4-5C4F-EF4A-AD84-6454213E0546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0231723D-D858-4647-8775-CC9D92E87CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="500" windowWidth="45080" windowHeight="26220" firstSheet="2" activeTab="12" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="-46420" yWindow="-4680" windowWidth="44800" windowHeight="26180" firstSheet="7" activeTab="14" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="adp1_antibiotic_10.12" sheetId="4" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="mgz1_mepMover_amp_2.4.23" sheetId="16" r:id="rId11"/>
     <sheet name="mgz1_DT_amp_2.7.23" sheetId="17" r:id="rId12"/>
     <sheet name="mgz1_3antibiotics_2.9.23" sheetId="18" r:id="rId13"/>
+    <sheet name="mgz1_cef_bia_2.25.23" sheetId="19" r:id="rId14"/>
+    <sheet name="nand_plasmid_amp_2.28.23" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5062" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5482" uniqueCount="138">
   <si>
     <t>well</t>
   </si>
@@ -449,6 +451,18 @@
   <si>
     <t>cefazolin</t>
   </si>
+  <si>
+    <t>MGZ1_dCasRx</t>
+  </si>
+  <si>
+    <t>MG1655</t>
+  </si>
+  <si>
+    <t>pJ2007_PhlF</t>
+  </si>
+  <si>
+    <t>pJ2007_IcaR</t>
+  </si>
 </sst>
 </file>
 
@@ -492,12 +506,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63BE7B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -512,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -522,6 +542,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9198,8 +9220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0316DAE-8BCC-A846-AB6B-A7C3C6D5DDFD}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11661,6 +11683,2144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE2A9F-CEC8-1043-A40C-B550A8586224}">
+  <dimension ref="A1:O19"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>5.5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>250</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>5.5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>250</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>5.5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>5.5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>5.5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>250</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>5.5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>250</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>5.5</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>250</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>5.5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>250</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>5.5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>250</v>
+      </c>
+      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>5.5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <v>250</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>5.5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>250</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>5.5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>5.5</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+      <c r="M14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>5.5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15">
+        <v>250</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>5.5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16">
+        <v>250</v>
+      </c>
+      <c r="M16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" t="s">
+        <v>102</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>5.5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>5.5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18">
+        <v>250</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>5.5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19">
+        <v>250</v>
+      </c>
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="E1:E19">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:I22">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:I13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40F125-1054-0F4A-B6CD-6BF39265F046}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>5.5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>250</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>5.5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>250</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>5.5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>5.5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>5.5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>250</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>5.5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>250</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>5.5</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>250</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>5.5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>250</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>5.5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>250</v>
+      </c>
+      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>5.5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <v>250</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>5.5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>250</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>5.5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>5.5</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+      <c r="M14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>5.5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15">
+        <v>250</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>5.5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16">
+        <v>250</v>
+      </c>
+      <c r="M16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" t="s">
+        <v>102</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>5.5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>5.5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18">
+        <v>250</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>5.5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19">
+        <v>250</v>
+      </c>
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <v>5.5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20">
+        <v>250</v>
+      </c>
+      <c r="M20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" t="s">
+        <v>102</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>5.5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21">
+        <v>250</v>
+      </c>
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>5.5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22">
+        <v>250</v>
+      </c>
+      <c r="M22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" t="s">
+        <v>102</v>
+      </c>
+      <c r="O22">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E8 E1 E15 E22">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:I15">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:I22">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E7">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F337F-D56F-DE4B-B44D-97EF61F12050}">
   <dimension ref="A1:K28"/>

</xml_diff>